<commit_message>
Removed buggy ingredient and repopulated the ingredient DB.
</commit_message>
<xml_diff>
--- a/JustNice2/data/Extracted.xlsx
+++ b/JustNice2/data/Extracted.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="471">
   <si>
     <t xml:space="preserve">Honey Mustard Grilled Chicken  </t>
   </si>
@@ -50,18 +50,9 @@
     <t>Place eggs in a medium saucepan and cover with cold water. Bring water to a boil and immediately remove from heat. Cover and let eggs stand in hot water for 10 to 12 minutes. Remove from hot water, cool and peel.**Slice eggs in half lengthwise. Remove yolks. Set aside whites.**In a medium bowl, mash egg yolks with a fork. Mix together with mayonnaise, shrimp, green onions, fresh dill weed, lime juice, prepared Dijon-style mustard, hot pepper sauce and ground black pepper.**Spoon approximately 1 tablespoon egg yolk mixture into each egg white. Garnish with fresh dill weed. Chill in the refrigerator until serving.**</t>
   </si>
   <si>
-    <t xml:space="preserve">Chile Cheese Squares  </t>
-  </si>
-  <si>
     <t>https://images.media-allrecipes.com/userphotos/560x315/1009327.jpg</t>
   </si>
   <si>
-    <t>Cheddar,Chile Pepper,Egg</t>
-  </si>
-  <si>
-    <t>Preheat oven to 350 degrees F (175 degrees C).**In a 9x13 inch baking dish, place 1/2 of the shredded Cheddar cheese. Top with green chile peppers. Top the  chiles with the remaining cheese.**In a blender, mix eggs with the juice from the chile peppers. Pour the egg mixture over the cheese mixture.**Bake in the preheated oven 30 to 40 minutes. Cool before cutting into squares.**</t>
-  </si>
-  <si>
     <t>https://images.media-allrecipes.com/userphotos/250x250/422820.jpg</t>
   </si>
   <si>
@@ -281,9 +272,6 @@
     <t>https://images.media-allrecipes.com/userphotos/560x315/712487.jpg</t>
   </si>
   <si>
-    <t>Potato,Bell Pepper,Chile,Salt,Black Pepper,Paprika,Vegetable Oil,Water</t>
-  </si>
-  <si>
     <t>In a saucepan, fry potatoes in oil until golden brown.**Stir in peppers, water, and seasonings.  Cover, and simmer until potatoes are tender.**</t>
   </si>
   <si>
@@ -740,9 +728,6 @@
     <t>https://images.media-allrecipes.com/userphotos/250x250/57432.jpg</t>
   </si>
   <si>
-    <t>Pea,Pepper,Onion,Chile Pepper,Pimento,Garlic,Salad Dressing</t>
-  </si>
-  <si>
     <t>In a mixing bowl, combine the black-eyed peas, green chili pepper, onion, jalapeno pepper, pimento, garlic and Italian-style dressing. Chill the mixture overnight.**</t>
   </si>
   <si>
@@ -1428,6 +1413,30 @@
   </si>
   <si>
     <t>rec_type</t>
+  </si>
+  <si>
+    <t>Western</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t>Preheat oven to 350 degrees F (175 degrees C).**In a 9x13 inch baking dish, place 1/2 of the shredded Cheddar cheese. Top with green chili peppers. Top the  chilis with the remaining cheese.**In a blender, mix eggs with the juice from the chili peppers. Pour the egg mixture over the cheese mixture.**Bake in the preheated oven 30 to 40 minutes. Cool before cutting into squares.**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chili Cheese Squares  </t>
+  </si>
+  <si>
+    <t>Cheddar,Chili Pepper,Egg</t>
+  </si>
+  <si>
+    <t>Potato,Bell Pepper,Chili,Salt,Black Pepper,Paprika,Vegetable Oil,Water</t>
+  </si>
+  <si>
+    <t>Pea,Pepper,Onion,Chili Pepper,Pimento,Garlic,Salad Dressing</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +1844,7 @@
   <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1850,28 +1859,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>467</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -1884,9 +1893,15 @@
       <c r="C2" s="7">
         <v>35</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="7">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>464</v>
+      </c>
       <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1904,9 +1919,15 @@
       <c r="C3" s="7">
         <v>50</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>465</v>
+      </c>
       <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1916,27 +1937,27 @@
     </row>
     <row r="4" spans="1:8" s="7" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>8</v>
+        <v>467</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>11</v>
+        <v>466</v>
       </c>
       <c r="C4" s="7">
         <v>50</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>10</v>
+        <v>468</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7">
         <v>810</v>
@@ -1945,18 +1966,18 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="7">
         <v>370</v>
@@ -1965,18 +1986,18 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="C7" s="7">
         <v>5</v>
@@ -1985,18 +2006,18 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="7">
         <v>185</v>
@@ -2005,18 +2026,18 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="C9" s="7">
         <v>5</v>
@@ -2025,35 +2046,35 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="7">
         <v>30</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="C11" s="7">
         <v>40</v>
@@ -2062,18 +2083,18 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="C12" s="7">
         <v>20</v>
@@ -2082,18 +2103,18 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="C13" s="7">
         <v>90</v>
@@ -2102,18 +2123,18 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="C14" s="7">
         <v>40</v>
@@ -2122,18 +2143,18 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="C15" s="7">
         <v>185</v>
@@ -2142,18 +2163,18 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="C16" s="7">
         <v>110</v>
@@ -2162,18 +2183,18 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="C17" s="7">
         <v>45</v>
@@ -2182,52 +2203,52 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="C18" s="7">
         <v>50</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="7" customFormat="1" ht="403.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="C19" s="7">
         <v>120</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="C20" s="7">
         <v>35</v>
@@ -2236,18 +2257,18 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="C21" s="7">
         <v>45</v>
@@ -2256,18 +2277,18 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C22" s="7">
         <v>55</v>
@@ -2276,18 +2297,18 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="C23" s="7">
         <v>5</v>
@@ -2296,69 +2317,69 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C24" s="7">
         <v>50</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>85</v>
+        <v>469</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C25" s="7">
         <v>45</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C26" s="7">
         <v>165</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C27" s="7">
         <v>5</v>
@@ -2367,52 +2388,52 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="7" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C28" s="7">
         <v>105</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C29" s="7">
         <v>200</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C30" s="7">
         <v>30</v>
@@ -2421,35 +2442,35 @@
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C31" s="7">
         <v>30</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C32" s="7">
         <v>80</v>
@@ -2458,137 +2479,137 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="7" customFormat="1" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C33" s="7">
         <v>40</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="7" customFormat="1" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C34" s="7">
         <v>105</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C35" s="7">
         <v>383</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C36" s="7">
         <v>55</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="7" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C37" s="7">
         <v>60</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C38" s="7">
         <v>75</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="7" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C39" s="7">
         <v>35</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C40" s="7">
         <v>30</v>
@@ -2597,18 +2618,18 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C41" s="7">
         <v>75</v>
@@ -2617,103 +2638,103 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C42" s="7">
         <v>60</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C43" s="7">
         <v>15</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C44" s="7">
         <v>40</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C45" s="7">
         <v>505</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="7" customFormat="1" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C46" s="7">
         <v>75</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="4" customFormat="1" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C47" s="7">
         <v>30</v>
@@ -2722,18 +2743,18 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C48" s="7">
         <v>30</v>
@@ -2742,18 +2763,18 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C49" s="7">
         <v>60</v>
@@ -2762,18 +2783,18 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="9" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C50" s="7">
         <v>100</v>
@@ -2782,35 +2803,35 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C51" s="7">
         <v>10</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C52" s="7">
         <v>20</v>
@@ -2819,18 +2840,18 @@
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C53" s="7">
         <v>12</v>
@@ -2839,18 +2860,18 @@
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C54" s="7">
         <v>15</v>
@@ -2859,18 +2880,18 @@
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C55" s="7">
         <v>15</v>
@@ -2879,18 +2900,18 @@
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="9" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C56" s="7">
         <v>812</v>
@@ -2899,18 +2920,18 @@
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="9" t="s">
-        <v>238</v>
+        <v>470</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C57" s="7">
         <v>15</v>
@@ -2919,18 +2940,18 @@
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="9" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C58" s="7">
         <v>130</v>
@@ -2939,52 +2960,52 @@
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="9" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C59" s="7">
         <v>105</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="7" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C60" s="7">
         <v>100</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C61" s="7">
         <v>30</v>
@@ -2993,18 +3014,18 @@
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C62" s="7">
         <v>80</v>
@@ -3013,35 +3034,35 @@
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="9" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="7" customFormat="1" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C63" s="7">
         <v>240</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C64" s="7">
         <v>20</v>
@@ -3050,69 +3071,69 @@
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="9" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C65" s="7">
         <v>40</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C66" s="7">
         <v>390</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="7" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C67" s="7">
         <v>70</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C68" s="7">
         <v>60</v>
@@ -3121,18 +3142,18 @@
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="9" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C69" s="7">
         <v>140</v>
@@ -3141,18 +3162,18 @@
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
       <c r="G69" s="9" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="7" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C70" s="7">
         <v>185</v>
@@ -3161,35 +3182,35 @@
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
       <c r="G70" s="9" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="7" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C71" s="7">
         <v>75</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="7" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C72" s="7">
         <v>30</v>
@@ -3198,52 +3219,52 @@
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="G72" s="9" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="7" customFormat="1" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="7" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C73" s="7">
         <v>120</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C74" s="7">
         <v>35</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="7" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C75" s="7">
         <v>30</v>
@@ -3252,18 +3273,18 @@
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="9" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C76" s="7">
         <v>75</v>
@@ -3272,18 +3293,18 @@
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="9" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="10" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C77" s="10">
         <v>150</v>
@@ -3292,18 +3313,18 @@
       <c r="E77" s="10"/>
       <c r="F77" s="10"/>
       <c r="G77" s="12" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="7" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C78" s="7">
         <v>160</v>
@@ -3312,18 +3333,18 @@
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="9" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="7" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C79" s="7">
         <v>90</v>
@@ -3332,18 +3353,18 @@
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="7" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C80" s="7">
         <v>5</v>
@@ -3352,18 +3373,18 @@
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="9" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="7" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C81" s="7">
         <v>25</v>
@@ -3372,18 +3393,18 @@
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
       <c r="G81" s="9" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="7" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C82" s="7">
         <v>70</v>
@@ -3392,35 +3413,35 @@
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
       <c r="G82" s="9" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="7" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C83" s="7">
         <v>100</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C84" s="4">
         <v>90</v>
@@ -3429,18 +3450,18 @@
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="6" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C85" s="4">
         <v>30</v>
@@ -3449,35 +3470,35 @@
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="6" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C86" s="4">
         <v>35</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="4" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C87" s="4">
         <v>17</v>
@@ -3486,18 +3507,18 @@
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="6" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C88" s="4">
         <v>15</v>
@@ -3506,18 +3527,18 @@
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C89" s="4">
         <v>60</v>
@@ -3526,35 +3547,35 @@
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
       <c r="G89" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C90" s="4">
         <v>40</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="7" customFormat="1" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C91" s="4">
         <v>80</v>
@@ -3563,18 +3584,18 @@
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C92" s="4">
         <v>100</v>
@@ -3583,18 +3604,18 @@
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="G92" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C93" s="4">
         <v>150</v>
@@ -3603,18 +3624,18 @@
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="6" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C94" s="4">
         <v>55</v>
@@ -3623,18 +3644,18 @@
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="6" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C95" s="4">
         <v>30</v>
@@ -3643,18 +3664,18 @@
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
       <c r="G95" s="6" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="7" customFormat="1" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="4" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C96" s="4">
         <v>50</v>
@@ -3663,35 +3684,35 @@
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
       <c r="G96" s="6" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="97" spans="1:8" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="4" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C97" s="4">
         <v>50</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C98" s="4">
         <v>35</v>
@@ -3700,18 +3721,18 @@
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
       <c r="G98" s="6" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C99" s="4">
         <v>10</v>
@@ -3720,35 +3741,35 @@
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
       <c r="G99" s="6" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="100" spans="1:8" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="4" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C100" s="4">
         <v>45</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="4" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C101" s="4">
         <v>55</v>
@@ -3757,18 +3778,18 @@
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
       <c r="G101" s="6" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="4" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C102" s="4">
         <v>45</v>
@@ -3777,35 +3798,35 @@
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
       <c r="G102" s="6" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="1:8" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="4" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C103" s="4">
         <v>35</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="3" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="4" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C104" s="4">
         <v>75</v>
@@ -3814,52 +3835,52 @@
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
       <c r="G104" s="6" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="4" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C105" s="4">
         <v>45</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="4" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C106" s="4">
         <v>75</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="7" customFormat="1" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="4" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C107" s="4">
         <v>70</v>
@@ -3868,35 +3889,35 @@
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="6" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="4" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C108" s="4">
         <v>5</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="4" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C109" s="4">
         <v>105</v>
@@ -3905,35 +3926,35 @@
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
       <c r="G109" s="6" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="4" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C110" s="4">
         <v>60</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="4" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C111" s="4">
         <v>95</v>
@@ -3942,35 +3963,35 @@
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="6" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="112" spans="1:8" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="4" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C112" s="4">
         <v>45</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="4" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C113" s="4">
         <v>60</v>
@@ -3979,18 +4000,18 @@
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="6" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="4" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C114" s="4">
         <v>370</v>
@@ -3999,18 +4020,18 @@
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="6" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="4" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C115" s="4">
         <v>55</v>
@@ -4019,18 +4040,18 @@
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="6" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="4" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C116" s="4">
         <v>30</v>
@@ -4039,10 +4060,10 @@
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
       <c r="G116" s="6" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -4164,5 +4185,6 @@
     <hyperlink ref="H53" r:id="rId115"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId116"/>
 </worksheet>
 </file>
</xml_diff>